<commit_message>
Updated DESeq BarPlot Titles
</commit_message>
<xml_diff>
--- a/DESEq2/All_Genus_Comparisons.xlsx
+++ b/DESEq2/All_Genus_Comparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caydenyu/Documents/GitHub/MICB-475-Team-2/DESEq2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970E8522-CE1F-234B-A60E-44C0262A0428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EF6876-0958-C44F-8DCB-6A0AA1233AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="3" xr2:uid="{3B31DE42-D7EE-3A4C-8F70-F78CCBE442D1}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{3B31DE42-D7EE-3A4C-8F70-F78CCBE442D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Group 3" sheetId="1" r:id="rId1"/>
@@ -449,14 +449,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7302400-33AB-7E47-8BC0-B6FDC77AFCB0}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,18 +804,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -844,7 +844,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2">
@@ -856,7 +856,7 @@
       <c r="D3" s="3">
         <v>6.4606798531222096E-7</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="2">
@@ -870,7 +870,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2">
@@ -882,7 +882,7 @@
       <c r="D4" s="3">
         <v>7.1338944724478702E-6</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="2">
@@ -896,7 +896,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2">
@@ -922,7 +922,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2">
@@ -934,7 +934,7 @@
       <c r="D6" s="2">
         <v>5.3291528200435998E-4</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="2">
@@ -948,7 +948,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2">
@@ -960,7 +960,7 @@
       <c r="D7" s="3">
         <v>5.12348007419835E-5</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="2">
@@ -1116,7 +1116,7 @@
       <c r="D13" s="2">
         <v>2.8974313909907101E-3</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="2">
@@ -1428,7 +1428,7 @@
       <c r="D25" s="2">
         <v>7.9416047445928905E-3</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G25" s="2">
@@ -1584,7 +1584,7 @@
       <c r="D31" s="2">
         <v>1.9302729225892501E-4</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="5" t="s">
         <v>17</v>
       </c>
       <c r="G31" s="2">
@@ -1610,7 +1610,7 @@
       <c r="D32" s="2">
         <v>5.6872288322624704E-4</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="4" t="s">
         <v>41</v>
       </c>
       <c r="G32" s="2">
@@ -1636,7 +1636,7 @@
       <c r="D33" s="2">
         <v>1.3352313427780001E-4</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="4" t="s">
         <v>43</v>
       </c>
       <c r="G33" s="2">
@@ -1692,7 +1692,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B37" s="2">
@@ -1706,7 +1706,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B38" s="2">
@@ -1734,7 +1734,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B40" s="2">
@@ -1762,7 +1762,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B42" s="2">
@@ -1776,7 +1776,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B43" s="2">
@@ -1802,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE215351-F860-D24B-AD60-269280747D2D}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="174" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="174" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1813,18 +1813,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1853,7 +1853,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2">
@@ -1865,7 +1865,7 @@
       <c r="D3" s="3">
         <v>7.2500080268111599E-11</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="2">
@@ -1879,7 +1879,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="2">
@@ -1891,7 +1891,7 @@
       <c r="D4" s="3">
         <v>2.0236457244334698E-9</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>27</v>
       </c>
       <c r="G4" s="2">
@@ -1905,7 +1905,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="2">
@@ -1917,7 +1917,7 @@
       <c r="D5" s="3">
         <v>2.5621728026511E-11</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="2">
@@ -1931,7 +1931,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="2">
@@ -1943,7 +1943,7 @@
       <c r="D6" s="3">
         <v>1.51201636515591E-5</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>53</v>
       </c>
       <c r="G6" s="2">
@@ -2009,7 +2009,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="2">
@@ -2035,7 +2035,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2">
@@ -2047,7 +2047,7 @@
       <c r="D10" s="3">
         <v>1.6685542038509401E-5</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>54</v>
       </c>
       <c r="G10" s="2">
@@ -2073,7 +2073,7 @@
       <c r="D11" s="3">
         <v>1.1512545714954001E-6</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="2">
@@ -2139,7 +2139,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="2">
@@ -2385,7 +2385,7 @@
       <c r="D23" s="3">
         <v>4.2054243706828502E-5</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G23" s="2">
@@ -3243,7 +3243,7 @@
       <c r="D56" s="3">
         <v>1.4602231794687401E-5</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="4" t="s">
         <v>81</v>
       </c>
       <c r="G56" s="2">
@@ -3271,7 +3271,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B58" s="2">
@@ -3325,8 +3325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EA921D-8882-F748-9420-286801554275}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView zoomScale="167" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3336,18 +3336,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3376,7 +3376,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="2">
@@ -3402,7 +3402,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2">
@@ -3414,7 +3414,7 @@
       <c r="D4" s="3">
         <v>3.0783512002036501E-6</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="2">
@@ -3454,7 +3454,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2">
@@ -3480,7 +3480,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="2">
@@ -3492,7 +3492,7 @@
       <c r="D7" s="3">
         <v>2.4499541620531001E-5</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="2">
@@ -3518,7 +3518,7 @@
       <c r="D8" s="3">
         <v>6.7505558814275201E-6</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="2">
@@ -3570,7 +3570,7 @@
       <c r="D10" s="2">
         <v>1.0201441166991501E-3</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>53</v>
       </c>
       <c r="G10" s="2">
@@ -4220,7 +4220,7 @@
       <c r="D35" s="2">
         <v>4.6449383825132497E-4</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="4" t="s">
         <v>60</v>
       </c>
       <c r="G35" s="2">
@@ -4234,7 +4234,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B36" s="2">
@@ -4260,8 +4260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E727795E-1B2E-DE45-881E-8E120A9FC885}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4271,18 +4271,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -4311,7 +4311,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2">
@@ -4323,7 +4323,7 @@
       <c r="D3" s="3">
         <v>3.3658296984176999E-6</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="2">
@@ -4337,7 +4337,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="2">
@@ -4349,7 +4349,7 @@
       <c r="D4" s="2">
         <v>3.5570423672412598E-3</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>27</v>
       </c>
       <c r="G4" s="2">
@@ -4363,7 +4363,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B5" s="2">
@@ -4375,7 +4375,7 @@
       <c r="D5" s="2">
         <v>5.7655996950315104E-3</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>54</v>
       </c>
       <c r="G5" s="2">
@@ -4389,7 +4389,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>68</v>
       </c>
       <c r="B6" s="2">
@@ -4427,7 +4427,7 @@
       <c r="D7" s="2">
         <v>7.9051942720014794E-3</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>68</v>
       </c>
       <c r="G7" s="2">

</xml_diff>

<commit_message>
updated volcano plot titles
</commit_message>
<xml_diff>
--- a/DESEq2/All_Genus_Comparisons.xlsx
+++ b/DESEq2/All_Genus_Comparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caydenyu/Documents/GitHub/MICB-475-Team-2/DESEq2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE482772-0B77-C944-AEC9-D19CBB492347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E74DC3-5059-F742-9A19-C774B6275CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="2" xr2:uid="{3B31DE42-D7EE-3A4C-8F70-F78CCBE442D1}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="3" xr2:uid="{3B31DE42-D7EE-3A4C-8F70-F78CCBE442D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Group 3" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Group 5" sheetId="3" r:id="rId3"/>
     <sheet name="Group 6" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="119">
   <si>
     <t>Genus</t>
   </si>
@@ -366,6 +366,36 @@
   </si>
   <si>
     <t>6 vs 2</t>
+  </si>
+  <si>
+    <t>Entacapone vs Healthy</t>
+  </si>
+  <si>
+    <t>Entacapone vs PD-untreated</t>
+  </si>
+  <si>
+    <t>Upregulated</t>
+  </si>
+  <si>
+    <t>Downregulated</t>
+  </si>
+  <si>
+    <t>Pramipexole vs Healthy</t>
+  </si>
+  <si>
+    <t>Pramipexole vs PD-untreated</t>
+  </si>
+  <si>
+    <t>Rasagiline vs Healthy</t>
+  </si>
+  <si>
+    <t>Rasagiline vs PD-untreated</t>
+  </si>
+  <si>
+    <t>Amantadine vs Healthy</t>
+  </si>
+  <si>
+    <t>Amantadine vs PD-untreated</t>
   </si>
 </sst>
 </file>
@@ -481,10 +511,10 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7302400-33AB-7E47-8BC0-B6FDC77AFCB0}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="A38" zoomScale="176" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -832,18 +862,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1815,6 +1845,40 @@
       </c>
       <c r="D43" s="3">
         <v>1.8951619650183801E-8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48">
+        <f>COUNTIF(B3:B43,"&gt;0")</f>
+        <v>16</v>
+      </c>
+      <c r="C48">
+        <f>COUNTIF(B3:B43,"&lt;0")</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49">
+        <f>COUNTIF(G3:G33,"&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="C49">
+        <f>COUNTIF(G3:G33,"&lt;0")</f>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1828,10 +1892,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE215351-F860-D24B-AD60-269280747D2D}">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A60" zoomScale="308" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1841,18 +1905,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3338,6 +3402,40 @@
       </c>
       <c r="D60" s="3">
         <v>4.8967276833309398E-8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>111</v>
+      </c>
+      <c r="C65" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66">
+        <f>COUNTIF(B3:B60,"&gt;0")</f>
+        <v>13</v>
+      </c>
+      <c r="C66">
+        <f>COUNTIF(B3:B60,"&lt;0")</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>114</v>
+      </c>
+      <c r="B67">
+        <f>COUNTIF(G3:G56,"&gt;0")</f>
+        <v>3</v>
+      </c>
+      <c r="C67">
+        <f>COUNTIF(G3:G56,"&lt;0")</f>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3351,10 +3449,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EA921D-8882-F748-9420-286801554275}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A15" zoomScale="142" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3364,18 +3462,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3534,7 +3632,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2">
@@ -4170,7 +4268,7 @@
       <c r="D32" s="2">
         <v>1.86679882422626E-3</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="12" t="s">
         <v>4</v>
       </c>
       <c r="G32" s="2">
@@ -4273,6 +4371,40 @@
       </c>
       <c r="D36" s="3">
         <v>5.65233045747078E-14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40">
+        <f>COUNTIF(B3:B36,"&gt;0")</f>
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <f>COUNTIF(B3:B36,"&lt;0")</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41">
+        <f>COUNTIF(G3:G35,"&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <f>COUNTIF(G3:G35,"&lt;0")</f>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -4286,10 +4418,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E727795E-1B2E-DE45-881E-8E120A9FC885}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4299,18 +4431,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -4544,6 +4676,40 @@
       </c>
       <c r="I10" s="2">
         <v>9.5056246625662907E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17">
+        <f>COUNTIF(B3:B10,"&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <f>COUNTIF(B3:B10,"&lt;0")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18">
+        <f>COUNTIF(G3:G10,"&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <f>COUNTIF(G3:G10,"&lt;0")</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>